<commit_message>
learnt some what-if analysis- Goal seeker, data tabel
</commit_message>
<xml_diff>
--- a/excel for dummies/Chapter02.xlsx
+++ b/excel for dummies/Chapter02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1777c78eef3b74d/Excel Data Analysis FD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knamas/Documents/Excel_For_Data_Analysis/excel for dummies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="861" documentId="8_{F97F57CE-6F09-45A5-92D2-B23FA5DCBC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{124ACD9E-DFE5-405D-9008-02A065C981CB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292774BD-E9A0-E249-99CB-BA48CC244250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="750" windowWidth="15330" windowHeight="10770" tabRatio="397" xr2:uid="{B9D60294-5061-4079-A876-B62BCD1CF08A}"/>
+    <workbookView xWindow="11520" yWindow="2360" windowWidth="28000" windowHeight="20260" tabRatio="397" activeTab="3" xr2:uid="{B9D60294-5061-4079-A876-B62BCD1CF08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Data Table" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -147,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Loan Payment Analysis</t>
   </si>
@@ -246,13 +244,79 @@
   </si>
   <si>
     <t>Total Profit</t>
+  </si>
+  <si>
+    <t>STEP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT B7:C15 </t>
+  </si>
+  <si>
+    <t>STEP2</t>
+  </si>
+  <si>
+    <t>DATA -&gt; WHAT -IF ANALYSIS -&gt; COLUMN CHOSSE : C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOU CAN SEE THAT THAT DIFFERENT DOLLAR AMOUNT WILL BE DISPLAYS ON THE SIDE </t>
+  </si>
+  <si>
+    <t>C8 TO C15 WAS EMPTY BEFORE THI CALCULATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT E7:F15 </t>
+  </si>
+  <si>
+    <t>YOU CAN SEE THAT THAT DIFFERENT DOLLAR AMOUNT WILL BE DISPLAYS ON THE SIDE BASED ON THE EARS CHANGE</t>
+  </si>
+  <si>
+    <t>DATA -&gt; WHAT -IF ANALYSIS -&gt; COLUMN CHOSSE : C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. SELECT DATA THAT YOU WANT TO DO WHAT-IF  ANALYSIS, IN THIS CASE B8:F:15 WHICH WAS BEOFRE </t>
+  </si>
+  <si>
+    <t>2. GO TO DATA -&gt; WHAT-IF-ANALYSIS- DATA TABLE</t>
+  </si>
+  <si>
+    <t>3. SELECT THE CELL YOU WANT CHANGE, IN THIS CASE I WANT TO CHANGE ROW FOR YEARS WHICH IS C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. SELECT THE CELL YOU WANT TO CHANG, IN THIS CASE I WANT TO CHANGE COLUMN FOR INTEREST RATEWHICH C2 </t>
+  </si>
+  <si>
+    <t>4. MAKE IS BOTH ROW AND COLABSOLUTE REFERENCE (LIKE $C$3)</t>
+  </si>
+  <si>
+    <t>1. YOU WANT TO SAVE 100000 IN 18YRS FOR YOUR KIDS COLLEGE EDUCATION AND YOU GET 4% INTEREST WHAT EVER YOUR INVEST THAT YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. GOTO DATA-&gt; WHAT-IF ANALYSIS -&gt; GOAL SEEK </t>
+  </si>
+  <si>
+    <t>3. SELECT SET CELL = THE AMOUNT YOU TO SAVE IN TOTAL IN THIS CASE B7</t>
+  </si>
+  <si>
+    <t>5. BY CHANGING CELL = HOW MUCH YOU WANT TO SAVE EVERYYEAR- HERE ANNUAL DEPOSIT</t>
+  </si>
+  <si>
+    <t>4. TO VALUE =  THE AMOUNT YOU WANT TO SAVE IN TOTAL, HERE COLLEGE REFUND CELL</t>
+  </si>
+  <si>
+    <t>6. BELOW IS THE CALCULATED CELLUSING ABOVE DETAILS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I didn’t do this sheet </t>
+  </si>
+  <si>
+    <t>I didn't understand the scenario manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
@@ -261,8 +325,9 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="\G\e\n\e\r\a\l"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -309,12 +374,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -474,7 +545,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -540,6 +611,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="5" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1275,28 +1354,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530417C6-67D8-4DD6-8966-E2CD0935EB7D}">
   <sheetPr published="0"/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
     <col min="3" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="12" width="8.83203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="24">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1304,7 +1385,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1320,7 +1401,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1328,73 +1409,196 @@
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="C7" s="6">
         <f>PMT(C2 / 12, C3 * 12, C4)</f>
         <v>-474.21131385767302</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8"/>
+      <c r="F7" s="6">
+        <f>PMT(C2 / 12, C3 * 12, C4)</f>
+        <v>-474.21131385767302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" s="7">
         <v>0.01</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <f t="dataTable" ref="C8:C15" dt2D="0" dtr="0" r1="C2" ca="1"/>
+        <v>-376.87245423055793</v>
+      </c>
       <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9"/>
+      <c r="E8" s="43">
+        <v>10</v>
+      </c>
+      <c r="F8" s="45">
+        <f t="dataTable" ref="F8:F15" dt2D="0" dtr="0" r1="C3"/>
+        <v>-965.60744698389522</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10"/>
+      <c r="C9" s="6">
+        <v>-399.93632623634915</v>
+      </c>
+      <c r="E9" s="43">
+        <v>15</v>
+      </c>
+      <c r="F9" s="46">
+        <v>-690.58164027799012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" s="7">
         <v>0.02</v>
       </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11"/>
+      <c r="C10" s="6">
+        <v>-423.85433864407338</v>
+      </c>
+      <c r="E10" s="43">
+        <v>20</v>
+      </c>
+      <c r="F10" s="46">
+        <v>-554.59759785391202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="B11" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12"/>
+      <c r="C11" s="6">
+        <v>-448.61673407662011</v>
+      </c>
+      <c r="E11" s="43">
+        <v>25</v>
+      </c>
+      <c r="F11" s="46">
+        <v>-474.21131385767302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="B12" s="7">
         <v>0.03</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13"/>
+      <c r="C12" s="6">
+        <v>-474.21131385767302</v>
+      </c>
+      <c r="E12" s="43">
+        <v>30</v>
+      </c>
+      <c r="F12" s="46">
+        <v>-421.60403372945046</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="B13" s="7">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="6">
+        <v>-500.62357025949291</v>
+      </c>
+      <c r="E13" s="43">
+        <v>35</v>
+      </c>
+      <c r="F13" s="46">
+        <v>-384.8501899407845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14"/>
       <c r="B14" s="7">
         <v>0.04</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="6">
+        <v>-527.83684029777737</v>
+      </c>
+      <c r="E14" s="44">
+        <v>40</v>
+      </c>
+      <c r="F14" s="46">
+        <v>-357.98442202873304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15"/>
       <c r="B15" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6">
+        <v>-614.08749228147019</v>
+      </c>
+      <c r="E15" s="44">
+        <v>45</v>
+      </c>
+      <c r="F15" s="46">
+        <v>-337.69060880752738</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="H17" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="H18" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="H19" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="47"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="J24" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1409,28 +1613,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F50C9B4-FE27-413B-B312-DDAC3AB1F73C}">
   <sheetPr published="0"/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B19" sqref="B19:K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
     <col min="3" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="24">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1438,7 +1642,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1446,7 +1650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1454,7 +1658,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1465,7 +1669,7 @@
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="B7" s="9">
         <f>PMT(C2 / 12, C3 * 12, C4)</f>
         <v>-474.21131385767302</v>
@@ -1483,87 +1687,234 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="7">
         <v>0.01</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="6">
+        <f t="dataTable" ref="C8:F15" dt2D="1" dtr="1" r1="C3" r2="C2"/>
+        <v>-598.4945145182694</v>
+      </c>
+      <c r="D8" s="6">
+        <v>-459.89430695779663</v>
+      </c>
+      <c r="E8" s="6">
+        <v>-376.87245423055793</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-321.63952044647004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="41"/>
       <c r="B9" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="6">
+        <v>-620.743020397431</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-482.54540888195254</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-399.93632623634915</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-345.12021045762697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="41"/>
       <c r="B10" s="7">
         <v>0.02</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="6">
+        <v>-643.50870055772566</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-505.88333504511718</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-423.85433864407338</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-369.61947268882057</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="41"/>
       <c r="B11" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="6">
+        <v>-666.7892090089864</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-529.90289303222994</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-448.61673407662011</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-395.12089881773204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="41"/>
       <c r="B12" s="7">
         <v>0.03</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="6">
+        <v>-690.58164027799012</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-554.59759785391202</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-474.21131385767302</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-421.60403372945046</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="41"/>
       <c r="B13" s="7">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="6">
+        <v>-714.88254134317515</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-579.95971798309336</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-500.62357025949291</v>
+      </c>
+      <c r="F13" s="6">
+        <v>-449.04468780882451</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="41"/>
       <c r="B14" s="7">
         <v>0.04</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="6">
+        <v>-739.68792560927022</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-605.98032929941871</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-527.83684029777737</v>
+      </c>
+      <c r="F14" s="6">
+        <v>-477.41529546545945</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="41"/>
       <c r="B15" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="6">
+        <v>-817.08345462113925</v>
+      </c>
+      <c r="D15" s="6">
+        <v>-687.8873078592386</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-614.08749228147019</v>
+      </c>
+      <c r="F15" s="6">
+        <v>-567.78900134700291</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1579,27 +1930,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61773C6-A337-4550-984E-FCE0E5D32A42}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="20.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="24">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
@@ -1607,7 +1958,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
@@ -1623,11 +1974,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" s="17"/>
       <c r="B6" s="16"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
@@ -1636,51 +1987,160 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
+      <c r="A12" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
+    </row>
+    <row r="21" spans="1:12" ht="24">
+      <c r="A21" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="16">
+        <v>-3899.3328144302432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="16">
+        <f>FV(B23,B24,B25)</f>
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1" gridLinesSet="0"/>
@@ -1695,33 +2155,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07CDA2B-7DD0-44B5-8D0E-30CCE5B44585}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="26">
       <c r="A1" s="42" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
@@ -1729,7 +2189,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -1737,12 +2197,12 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
@@ -1750,7 +2210,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
@@ -1758,7 +2218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
@@ -1766,7 +2226,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="34.5" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
@@ -1777,7 +2237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="19" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +2249,7 @@
         <v>-584.78426343953493</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
@@ -1801,7 +2261,7 @@
         <v>-106986.75295157434</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="19" t="s">
         <v>20</v>
       </c>
@@ -1814,7 +2274,7 @@
         <v>9361.4702739140339</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
@@ -1826,22 +2286,27 @@
         <v>15.245900588236969</v>
       </c>
     </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="47"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+    </row>
   </sheetData>
-  <scenarios current="0" show="1" sqref="B12:C13 C14 C15">
-    <scenario name="Best Case" count="3" user="Paul M" comment="Mortgage Analysis - Best Case Scenario:_x000a_ - maximum down payment_x000a_ - minimum term_x000a_ - maximum monthly paydown_x000a_">
-      <inputCells r="B7" val="20000" numFmtId="165"/>
+  <scenarios current="1" show="0" sqref="B12:C13 C14 C15">
+    <scenario name="Best Case" count="3" user="Microsoft Office User" comment="Mortgage Analysis - Best Case Scenario:_x000a_ - maximum down Payment_x000a_ - minimum term_x000a_ - maximum monthly paydown_x000a_">
+      <inputCells r="B7" val="20000" numFmtId="6"/>
       <inputCells r="B8" val="20"/>
-      <inputCells r="B9" val="-100" numFmtId="164"/>
+      <inputCells r="B9" val="-100" numFmtId="5"/>
     </scenario>
-    <scenario name="Worst Case" locked="1" count="3" user="Paul McFedries" comment="Mortgage Analysis - Worst Case Scenario_x000a_ - minimum down payment_x000a_ - maximum term_x000a_ - no monthly paydown">
-      <inputCells r="B7" val="10000" numFmtId="165"/>
-      <inputCells r="B8" val="30"/>
-      <inputCells r="B9" val="0" numFmtId="164"/>
-    </scenario>
-    <scenario name="Likeliest Case" locked="1" count="3" user="Paul M" comment="Mortgage Analysis - Likliest Case Scenario:_x000a_ - average down payment_x000a_ - average term_x000a_ - average monthly paydown_x000a_Modified by Paul M on 11/12/2012">
-      <inputCells r="B7" val="15000" numFmtId="165"/>
+    <scenario name="middle case" count="3" user="Microsoft Office User">
+      <inputCells r="B7" val="20000" numFmtId="6"/>
       <inputCells r="B8" val="25"/>
-      <inputCells r="B9" val="-50" numFmtId="164"/>
+      <inputCells r="B9" val="-100" numFmtId="5"/>
     </scenario>
   </scenarios>
   <mergeCells count="1">
@@ -1858,22 +2323,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED213781-706E-4C84-BD68-F22D4D3AE53C}">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="40">
       <c r="A2" s="27"/>
       <c r="B2" s="28" t="s">
         <v>22</v>
@@ -1882,7 +2347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="29" t="s">
         <v>24</v>
       </c>
@@ -1893,7 +2358,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="31" t="s">
         <v>25</v>
       </c>
@@ -1904,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="31" t="s">
         <v>26</v>
       </c>
@@ -1917,12 +2382,12 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="29"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="29" t="s">
         <v>27</v>
       </c>
@@ -1933,7 +2398,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="29" t="s">
         <v>28</v>
       </c>
@@ -1946,7 +2411,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="31" t="s">
         <v>29</v>
       </c>
@@ -1957,7 +2422,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="31" t="s">
         <v>30</v>
       </c>
@@ -1970,12 +2435,12 @@
         <v>75008.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="29"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
     </row>
-    <row r="12" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="20" thickBot="1">
       <c r="A12" s="36" t="s">
         <v>31</v>
       </c>
@@ -1988,11 +2453,11 @@
         <v>-74988.55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="20" thickBot="1">
       <c r="A14" s="36" t="s">
         <v>32</v>
       </c>
@@ -2001,6 +2466,11 @@
         <v>-174975.1</v>
       </c>
       <c r="C14" s="4"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="47" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <scenarios current="1">

</xml_diff>